<commit_message>
updated publications, talks, conferences.
</commit_message>
<xml_diff>
--- a/data/conference.xlsx
+++ b/data/conference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f7c762a89876f48/R/projects/jy_CV_original/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f7c762a89876f48/R/projects/cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{C90AD6C8-6BA7-554D-A94C-770A2C36C37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB00A1F1-1672-164F-96C3-8F076D2216F1}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="8_{C90AD6C8-6BA7-554D-A94C-770A2C36C37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFCC66D9-4060-404E-A9DF-C161B0DF5E57}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t>what</t>
   </si>
@@ -296,6 +296,18 @@
   </si>
   <si>
     <t>Ulaan Baatar</t>
+  </si>
+  <si>
+    <t>Korean Association for Public Diplomacy</t>
+  </si>
+  <si>
+    <t>2022 November</t>
+  </si>
+  <si>
+    <t>Public Diplomacy in Other Words</t>
+  </si>
+  <si>
+    <t>What Drives South Korea’s Covid-19 Humanitarian Aid?</t>
   </si>
 </sst>
 </file>
@@ -1189,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1226,112 +1238,107 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
-        <v>42</v>
+      <c r="A2" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" ht="16">
+    <row r="3" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="1"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="16">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="16">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="16">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="16">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>8</v>
@@ -1340,140 +1347,140 @@
     </row>
     <row r="9" spans="1:11" ht="16">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="16">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="16">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="16">
-      <c r="A12" s="7" t="s">
-        <v>38</v>
+      <c r="A12" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="K12" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="16">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="16">
-      <c r="A14" s="4" t="s">
-        <v>47</v>
+      <c r="A14" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="1"/>
+      <c r="E14" s="8"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="16">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="16">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>52</v>
+        <v>10</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="K16" s="1"/>
     </row>
@@ -1485,210 +1492,231 @@
         <v>51</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="E17" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="16">
       <c r="A18" s="4" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="16">
       <c r="A19" s="4" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K19" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="16">
       <c r="A20" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="16">
       <c r="A21" s="4" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="16">
       <c r="A22" s="4" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="16">
       <c r="A23" s="4" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="E23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="16">
       <c r="A24" s="4" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="16">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="16">
       <c r="A26" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="16">
       <c r="A27" s="4" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="16">
       <c r="A28" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="16">
       <c r="A29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" ht="16">
+      <c r="A30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" ht="16">
+      <c r="A31" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" ht="16">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" ht="16">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" ht="16">
       <c r="A32" s="5"/>
@@ -1736,6 +1764,7 @@
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" ht="16">
       <c r="A40" s="5"/>
@@ -1747,7 +1776,6 @@
       <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="16">
       <c r="A42" s="5"/>
@@ -1789,6 +1817,7 @@
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" ht="16">
       <c r="A49" s="5"/>
@@ -1800,7 +1829,6 @@
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" ht="16">
       <c r="A51" s="5"/>
@@ -1820,6 +1848,18 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
+    <row r="54" spans="1:4" ht="16">
+      <c r="A54" s="5"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4" ht="16">
+      <c r="A55" s="5"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>